<commit_message>
Adding index column in pandas reading
</commit_message>
<xml_diff>
--- a/hira-kata.xlsx
+++ b/hira-kata.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+  <si>
+    <t xml:space="preserve">idx</t>
+  </si>
   <si>
     <t xml:space="preserve">hiragana</t>
   </si>
@@ -223,7 +226,7 @@
     <t xml:space="preserve">ナ</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">Na</t>
   </si>
   <si>
     <t xml:space="preserve">に</t>
@@ -577,44 +580,47 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F50" activeCellId="0" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.87854251012146"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -623,18 +629,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -643,18 +649,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -663,18 +669,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -683,18 +689,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
@@ -703,18 +709,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -723,18 +729,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
@@ -743,18 +749,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
@@ -763,18 +769,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
@@ -783,18 +789,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
@@ -803,18 +809,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
@@ -823,18 +829,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
@@ -843,18 +849,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -863,18 +869,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -883,18 +889,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -903,18 +909,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -923,18 +929,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -943,18 +949,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -963,18 +969,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -983,18 +989,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -1003,18 +1009,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -1023,18 +1029,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -1043,18 +1049,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -1063,18 +1069,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -1083,18 +1089,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
@@ -1103,18 +1109,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
@@ -1123,18 +1129,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
@@ -1143,18 +1149,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
@@ -1163,18 +1169,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1</v>
@@ -1183,18 +1189,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
@@ -1203,18 +1209,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
@@ -1223,18 +1229,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
@@ -1243,18 +1249,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
@@ -1263,18 +1269,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -1283,18 +1289,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
@@ -1303,18 +1309,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
@@ -1323,18 +1329,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
@@ -1343,18 +1349,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>1</v>
@@ -1363,18 +1369,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1</v>
@@ -1383,18 +1389,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
@@ -1403,18 +1409,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>1</v>
@@ -1423,18 +1429,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1</v>
@@ -1443,18 +1449,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
@@ -1463,18 +1469,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
@@ -1483,18 +1489,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1</v>
@@ -1503,18 +1509,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>1</v>

</xml_diff>